<commit_message>
only search for keyword inside the law text, not the entire page
</commit_message>
<xml_diff>
--- a/laws-data.xlsx
+++ b/laws-data.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E259"/>
+  <dimension ref="A1:G259"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -418,6 +418,12 @@
       <c r="E1" t="str">
         <v>Bộ Công an</v>
       </c>
+      <c r="F1" t="str">
+        <v>ban hành</v>
+      </c>
+      <c r="G1" t="str">
+        <v>điều tra</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -429,6 +435,12 @@
       <c r="E2">
         <v>0</v>
       </c>
+      <c r="F2">
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
@@ -446,6 +458,12 @@
       <c r="E3">
         <v>16</v>
       </c>
+      <c r="F3">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>43</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
@@ -463,6 +481,12 @@
       <c r="E4">
         <v>0</v>
       </c>
+      <c r="F4">
+        <v>16</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="str">
@@ -480,6 +504,12 @@
       <c r="E5">
         <v>0</v>
       </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="str">
@@ -497,6 +527,12 @@
       <c r="E6">
         <v>14</v>
       </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="str">
@@ -514,6 +550,12 @@
       <c r="E7">
         <v>0</v>
       </c>
+      <c r="F7">
+        <v>8</v>
+      </c>
+      <c r="G7">
+        <v>4</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="str">
@@ -531,6 +573,12 @@
       <c r="E8">
         <v>2</v>
       </c>
+      <c r="F8">
+        <v>21</v>
+      </c>
+      <c r="G8">
+        <v>36</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="str">
@@ -546,7 +594,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Quyen-dan-su/Luat-Can-cuoc-26-2023-QH15-552422.aspx</v>
       </c>
       <c r="E9">
-        <v>22</v>
+        <v>21</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -565,6 +619,12 @@
       <c r="E10">
         <v>18</v>
       </c>
+      <c r="F10">
+        <v>41</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="str">
@@ -582,6 +642,12 @@
       <c r="E11">
         <v>3</v>
       </c>
+      <c r="F11">
+        <v>12</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="str">
@@ -599,6 +665,12 @@
       <c r="E12">
         <v>0</v>
       </c>
+      <c r="F12">
+        <v>10</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="str">
@@ -616,6 +688,12 @@
       <c r="E13">
         <v>3</v>
       </c>
+      <c r="F13">
+        <v>34</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="str">
@@ -633,6 +711,12 @@
       <c r="E14">
         <v>0</v>
       </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="str">
@@ -650,6 +734,12 @@
       <c r="E15">
         <v>0</v>
       </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="str">
@@ -667,6 +757,12 @@
       <c r="E16">
         <v>2</v>
       </c>
+      <c r="F16">
+        <v>47</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="str">
@@ -682,7 +778,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Quyen-dan-su/Luat-Xuat-canh-nhap-canh-cong-dan-Viet-Nam-va-Luat-Nhap-canh-nguoi-nuoc-ngoai-sua-doi-2023-563579.aspx</v>
       </c>
       <c r="E17">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -701,6 +803,12 @@
       <c r="E18">
         <v>0</v>
       </c>
+      <c r="F18">
+        <v>19</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="str">
@@ -716,7 +824,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Bo-may-hanh-chinh/Luat-Cong-an-nhan-dan-sua-doi-2023-21-2023-QH15-552424.aspx</v>
       </c>
       <c r="E19">
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -735,6 +849,12 @@
       <c r="E20">
         <v>5</v>
       </c>
+      <c r="F20">
+        <v>14</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="str">
@@ -752,6 +872,12 @@
       <c r="E21">
         <v>4</v>
       </c>
+      <c r="F21">
+        <v>9</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="str">
@@ -769,6 +895,12 @@
       <c r="E22">
         <v>0</v>
       </c>
+      <c r="F22">
+        <v>56</v>
+      </c>
+      <c r="G22">
+        <v>14</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="str">
@@ -786,6 +918,12 @@
       <c r="E23">
         <v>0</v>
       </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>81</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="str">
@@ -803,6 +941,12 @@
       <c r="E24">
         <v>1</v>
       </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
@@ -820,6 +964,12 @@
       <c r="E25">
         <v>1</v>
       </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
@@ -837,6 +987,12 @@
       <c r="E26">
         <v>9</v>
       </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
@@ -854,6 +1010,12 @@
       <c r="E27">
         <v>0</v>
       </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
@@ -871,6 +1033,12 @@
       <c r="E28">
         <v>0</v>
       </c>
+      <c r="F28">
+        <v>6</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
@@ -888,6 +1056,12 @@
       <c r="E29">
         <v>23</v>
       </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
@@ -905,6 +1079,12 @@
       <c r="E30">
         <v>1</v>
       </c>
+      <c r="F30">
+        <v>7</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
@@ -922,6 +1102,12 @@
       <c r="E31">
         <v>17</v>
       </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
@@ -939,6 +1125,12 @@
       <c r="E32">
         <v>0</v>
       </c>
+      <c r="F32">
+        <v>1</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
@@ -956,6 +1148,12 @@
       <c r="E33">
         <v>0</v>
       </c>
+      <c r="F33">
+        <v>6</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
@@ -973,6 +1171,12 @@
       <c r="E34">
         <v>3</v>
       </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>5</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
@@ -990,6 +1194,12 @@
       <c r="E35">
         <v>2</v>
       </c>
+      <c r="F35">
+        <v>12</v>
+      </c>
+      <c r="G35">
+        <v>2</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
@@ -1007,6 +1217,12 @@
       <c r="E36">
         <v>6</v>
       </c>
+      <c r="F36">
+        <v>70</v>
+      </c>
+      <c r="G36">
+        <v>12</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
@@ -1024,6 +1240,12 @@
       <c r="E37">
         <v>0</v>
       </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="str">
@@ -1041,6 +1263,12 @@
       <c r="E38">
         <v>0</v>
       </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="str">
@@ -1058,6 +1286,12 @@
       <c r="E39">
         <v>6</v>
       </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="str">
@@ -1075,6 +1309,12 @@
       <c r="E40">
         <v>0</v>
       </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>25</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="str">
@@ -1092,6 +1332,12 @@
       <c r="E41">
         <v>3</v>
       </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="str">
@@ -1109,6 +1355,12 @@
       <c r="E42">
         <v>3</v>
       </c>
+      <c r="F42">
+        <v>9</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="str">
@@ -1126,6 +1378,12 @@
       <c r="E43">
         <v>0</v>
       </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="str">
@@ -1143,6 +1401,12 @@
       <c r="E44">
         <v>0</v>
       </c>
+      <c r="F44">
+        <v>57</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="str">
@@ -1160,6 +1424,12 @@
       <c r="E45">
         <v>1</v>
       </c>
+      <c r="F45">
+        <v>14</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="str">
@@ -1177,6 +1447,12 @@
       <c r="E46">
         <v>0</v>
       </c>
+      <c r="F46">
+        <v>9</v>
+      </c>
+      <c r="G46">
+        <v>6</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="str">
@@ -1194,6 +1470,12 @@
       <c r="E47">
         <v>2</v>
       </c>
+      <c r="F47">
+        <v>19</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="str">
@@ -1211,6 +1493,12 @@
       <c r="E48">
         <v>0</v>
       </c>
+      <c r="F48">
+        <v>5</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="str">
@@ -1226,7 +1514,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Doanh-nghiep/Luat-Dau-tu-so-61-2020-QH14-321051.aspx</v>
       </c>
       <c r="E49">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>15</v>
+      </c>
+      <c r="G49">
+        <v>2</v>
       </c>
     </row>
     <row r="50">
@@ -1245,6 +1539,12 @@
       <c r="E50">
         <v>0</v>
       </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="str">
@@ -1262,6 +1562,12 @@
       <c r="E51">
         <v>0</v>
       </c>
+      <c r="F51">
+        <v>11</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="str">
@@ -1279,6 +1585,12 @@
       <c r="E52">
         <v>4</v>
       </c>
+      <c r="F52">
+        <v>7</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="str">
@@ -1296,6 +1608,12 @@
       <c r="E53">
         <v>0</v>
       </c>
+      <c r="F53">
+        <v>3</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="str">
@@ -1313,6 +1631,12 @@
       <c r="E54">
         <v>0</v>
       </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="str">
@@ -1330,6 +1654,12 @@
       <c r="E55">
         <v>0</v>
       </c>
+      <c r="F55">
+        <v>16</v>
+      </c>
+      <c r="G55">
+        <v>3</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="str">
@@ -1347,6 +1677,12 @@
       <c r="E56">
         <v>1</v>
       </c>
+      <c r="F56">
+        <v>1</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="str">
@@ -1364,6 +1700,12 @@
       <c r="E57">
         <v>0</v>
       </c>
+      <c r="F57">
+        <v>2</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="str">
@@ -1381,6 +1723,12 @@
       <c r="E58">
         <v>0</v>
       </c>
+      <c r="F58">
+        <v>4</v>
+      </c>
+      <c r="G58">
+        <v>8</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="str">
@@ -1398,6 +1746,12 @@
       <c r="E59">
         <v>0</v>
       </c>
+      <c r="F59">
+        <v>1</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="str">
@@ -1415,6 +1769,12 @@
       <c r="E60">
         <v>53</v>
       </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="str">
@@ -1432,6 +1792,12 @@
       <c r="E61">
         <v>0</v>
       </c>
+      <c r="F61">
+        <v>9</v>
+      </c>
+      <c r="G61">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="str">
@@ -1449,6 +1815,12 @@
       <c r="E62">
         <v>1</v>
       </c>
+      <c r="F62">
+        <v>11</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="str">
@@ -1464,7 +1836,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Lao-dong-Tien-luong/Bo-Luat-lao-dong-2019-333670.aspx</v>
       </c>
       <c r="E63">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>16</v>
+      </c>
+      <c r="G63">
+        <v>3</v>
       </c>
     </row>
     <row r="64">
@@ -1483,6 +1861,12 @@
       <c r="E64">
         <v>73</v>
       </c>
+      <c r="F64">
+        <v>12</v>
+      </c>
+      <c r="G64">
+        <v>23</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="str">
@@ -1500,6 +1884,12 @@
       <c r="E65">
         <v>0</v>
       </c>
+      <c r="F65">
+        <v>3</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="str">
@@ -1517,6 +1907,12 @@
       <c r="E66">
         <v>0</v>
       </c>
+      <c r="F66">
+        <v>4</v>
+      </c>
+      <c r="G66">
+        <v>0</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="str">
@@ -1534,6 +1930,12 @@
       <c r="E67">
         <v>1</v>
       </c>
+      <c r="F67">
+        <v>14</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="str">
@@ -1551,6 +1953,12 @@
       <c r="E68">
         <v>0</v>
       </c>
+      <c r="F68">
+        <v>12</v>
+      </c>
+      <c r="G68">
+        <v>1</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="str">
@@ -1568,6 +1976,12 @@
       <c r="E69">
         <v>2</v>
       </c>
+      <c r="F69">
+        <v>13</v>
+      </c>
+      <c r="G69">
+        <v>12</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="str">
@@ -1585,6 +1999,12 @@
       <c r="E70">
         <v>0</v>
       </c>
+      <c r="F70">
+        <v>15</v>
+      </c>
+      <c r="G70">
+        <v>0</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="str">
@@ -1600,7 +2020,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Bo-may-hanh-chinh/Luat-Cong-an-nhan-dan-384487.aspx</v>
       </c>
       <c r="E71">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="F71">
+        <v>4</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
       </c>
     </row>
     <row r="72">
@@ -1619,6 +2045,12 @@
       <c r="E72">
         <v>3</v>
       </c>
+      <c r="F72">
+        <v>21</v>
+      </c>
+      <c r="G72">
+        <v>29</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="str">
@@ -1636,6 +2068,12 @@
       <c r="E73">
         <v>5</v>
       </c>
+      <c r="F73">
+        <v>19</v>
+      </c>
+      <c r="G73">
+        <v>18</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="str">
@@ -1653,6 +2091,12 @@
       <c r="E74">
         <v>23</v>
       </c>
+      <c r="F74">
+        <v>5</v>
+      </c>
+      <c r="G74">
+        <v>1</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="str">
@@ -1670,6 +2114,12 @@
       <c r="E75">
         <v>0</v>
       </c>
+      <c r="F75">
+        <v>12</v>
+      </c>
+      <c r="G75">
+        <v>3</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="str">
@@ -1687,6 +2137,12 @@
       <c r="E76">
         <v>1</v>
       </c>
+      <c r="F76">
+        <v>19</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="str">
@@ -1704,6 +2160,12 @@
       <c r="E77">
         <v>0</v>
       </c>
+      <c r="F77">
+        <v>18</v>
+      </c>
+      <c r="G77">
+        <v>4</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="str">
@@ -1721,6 +2183,12 @@
       <c r="E78">
         <v>0</v>
       </c>
+      <c r="F78">
+        <v>5</v>
+      </c>
+      <c r="G78">
+        <v>4</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="str">
@@ -1738,6 +2206,12 @@
       <c r="E79">
         <v>11</v>
       </c>
+      <c r="F79">
+        <v>15</v>
+      </c>
+      <c r="G79">
+        <v>2</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="str">
@@ -1755,6 +2229,12 @@
       <c r="E80">
         <v>0</v>
       </c>
+      <c r="F80">
+        <v>21</v>
+      </c>
+      <c r="G80">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="str">
@@ -1772,6 +2252,12 @@
       <c r="E81">
         <v>1</v>
       </c>
+      <c r="F81">
+        <v>17</v>
+      </c>
+      <c r="G81">
+        <v>1</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="str">
@@ -1789,6 +2275,12 @@
       <c r="E82">
         <v>2</v>
       </c>
+      <c r="F82">
+        <v>9</v>
+      </c>
+      <c r="G82">
+        <v>0</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="str">
@@ -1806,6 +2298,12 @@
       <c r="E83">
         <v>25</v>
       </c>
+      <c r="F83">
+        <v>6</v>
+      </c>
+      <c r="G83">
+        <v>4</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="str">
@@ -1823,6 +2321,12 @@
       <c r="E84">
         <v>0</v>
       </c>
+      <c r="F84">
+        <v>2</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="str">
@@ -1840,6 +2344,12 @@
       <c r="E85">
         <v>0</v>
       </c>
+      <c r="F85">
+        <v>5</v>
+      </c>
+      <c r="G85">
+        <v>205</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="str">
@@ -1857,6 +2367,12 @@
       <c r="E86">
         <v>2</v>
       </c>
+      <c r="F86">
+        <v>6</v>
+      </c>
+      <c r="G86">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="str">
@@ -1874,6 +2390,12 @@
       <c r="E87">
         <v>0</v>
       </c>
+      <c r="F87">
+        <v>23</v>
+      </c>
+      <c r="G87">
+        <v>3</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="str">
@@ -1891,6 +2413,12 @@
       <c r="E88">
         <v>0</v>
       </c>
+      <c r="F88">
+        <v>5</v>
+      </c>
+      <c r="G88">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="str">
@@ -1908,6 +2436,12 @@
       <c r="E89">
         <v>1</v>
       </c>
+      <c r="F89">
+        <v>23</v>
+      </c>
+      <c r="G89">
+        <v>33</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="str">
@@ -1925,6 +2459,12 @@
       <c r="E90">
         <v>0</v>
       </c>
+      <c r="F90">
+        <v>1</v>
+      </c>
+      <c r="G90">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="str">
@@ -1942,6 +2482,12 @@
       <c r="E91">
         <v>1</v>
       </c>
+      <c r="F91">
+        <v>12</v>
+      </c>
+      <c r="G91">
+        <v>18</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="str">
@@ -1959,6 +2505,12 @@
       <c r="E92">
         <v>6</v>
       </c>
+      <c r="F92">
+        <v>15</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="str">
@@ -1976,6 +2528,12 @@
       <c r="E93">
         <v>14</v>
       </c>
+      <c r="F93">
+        <v>6</v>
+      </c>
+      <c r="G93">
+        <v>0</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="str">
@@ -1991,7 +2549,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Linh-vuc-khac/Luat-Quan-ly-su-dung-vu-khi-vat-lieu-no-cong-cu-ho-tro-2017-320097.aspx</v>
       </c>
       <c r="E94">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="F94">
+        <v>9</v>
+      </c>
+      <c r="G94">
+        <v>5</v>
       </c>
     </row>
     <row r="95">
@@ -2010,6 +2574,12 @@
       <c r="E95">
         <v>1</v>
       </c>
+      <c r="F95">
+        <v>6</v>
+      </c>
+      <c r="G95">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="str">
@@ -2027,6 +2597,12 @@
       <c r="E96">
         <v>0</v>
       </c>
+      <c r="F96">
+        <v>11</v>
+      </c>
+      <c r="G96">
+        <v>39</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="str">
@@ -2044,6 +2620,12 @@
       <c r="E97">
         <v>0</v>
       </c>
+      <c r="F97">
+        <v>1</v>
+      </c>
+      <c r="G97">
+        <v>2</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="str">
@@ -2061,6 +2643,12 @@
       <c r="E98">
         <v>0</v>
       </c>
+      <c r="F98">
+        <v>16</v>
+      </c>
+      <c r="G98">
+        <v>3</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="str">
@@ -2078,6 +2666,12 @@
       <c r="E99">
         <v>0</v>
       </c>
+      <c r="F99">
+        <v>10</v>
+      </c>
+      <c r="G99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="str">
@@ -2095,6 +2689,12 @@
       <c r="E100">
         <v>0</v>
       </c>
+      <c r="F100">
+        <v>9</v>
+      </c>
+      <c r="G100">
+        <v>13</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="str">
@@ -2112,6 +2712,12 @@
       <c r="E101">
         <v>1</v>
       </c>
+      <c r="F101">
+        <v>4</v>
+      </c>
+      <c r="G101">
+        <v>2</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="str">
@@ -2129,6 +2735,12 @@
       <c r="E102">
         <v>0</v>
       </c>
+      <c r="F102">
+        <v>5</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="str">
@@ -2146,6 +2758,12 @@
       <c r="E103">
         <v>1</v>
       </c>
+      <c r="F103">
+        <v>13</v>
+      </c>
+      <c r="G103">
+        <v>174</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="str">
@@ -2163,6 +2781,12 @@
       <c r="E104">
         <v>0</v>
       </c>
+      <c r="F104">
+        <v>2</v>
+      </c>
+      <c r="G104">
+        <v>2</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="str">
@@ -2180,6 +2804,12 @@
       <c r="E105">
         <v>0</v>
       </c>
+      <c r="F105">
+        <v>2</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="str">
@@ -2197,6 +2827,12 @@
       <c r="E106">
         <v>0</v>
       </c>
+      <c r="F106">
+        <v>10</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="str">
@@ -2214,6 +2850,12 @@
       <c r="E107">
         <v>1</v>
       </c>
+      <c r="F107">
+        <v>16</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="str">
@@ -2231,6 +2873,12 @@
       <c r="E108">
         <v>0</v>
       </c>
+      <c r="F108">
+        <v>32</v>
+      </c>
+      <c r="G108">
+        <v>1</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="str">
@@ -2248,6 +2896,12 @@
       <c r="E109">
         <v>0</v>
       </c>
+      <c r="F109">
+        <v>4</v>
+      </c>
+      <c r="G109">
+        <v>5</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="str">
@@ -2265,6 +2919,12 @@
       <c r="E110">
         <v>0</v>
       </c>
+      <c r="F110">
+        <v>1</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="str">
@@ -2282,6 +2942,12 @@
       <c r="E111">
         <v>1</v>
       </c>
+      <c r="F111">
+        <v>5</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="str">
@@ -2299,6 +2965,12 @@
       <c r="E112">
         <v>1</v>
       </c>
+      <c r="F112">
+        <v>9</v>
+      </c>
+      <c r="G112">
+        <v>2</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="str">
@@ -2316,6 +2988,12 @@
       <c r="E113">
         <v>0</v>
       </c>
+      <c r="F113">
+        <v>3</v>
+      </c>
+      <c r="G113">
+        <v>5</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="str">
@@ -2333,6 +3011,12 @@
       <c r="E114">
         <v>8</v>
       </c>
+      <c r="F114">
+        <v>8</v>
+      </c>
+      <c r="G114">
+        <v>1049</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="str">
@@ -2348,6 +3032,12 @@
         <v>https://thuvienphapluat.vn/van-ban/Trach-nhiem-hinh-su/Bo-luat-hinh-su-2015-296661.aspx</v>
       </c>
       <c r="E115">
+        <v>0</v>
+      </c>
+      <c r="F115">
+        <v>2</v>
+      </c>
+      <c r="G115">
         <v>14</v>
       </c>
     </row>
@@ -2367,6 +3057,12 @@
       <c r="E116">
         <v>0</v>
       </c>
+      <c r="F116">
+        <v>3</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="str">
@@ -2382,7 +3078,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Trach-nhiem-hinh-su/Luat-to-chuc-co-quan-dieu-tra-hinh-su-2015-298378.aspx</v>
       </c>
       <c r="E117">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="F117">
+        <v>9</v>
+      </c>
+      <c r="G117">
+        <v>525</v>
       </c>
     </row>
     <row r="118">
@@ -2401,6 +3103,12 @@
       <c r="E118">
         <v>0</v>
       </c>
+      <c r="F118">
+        <v>13</v>
+      </c>
+      <c r="G118">
+        <v>1</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="str">
@@ -2418,6 +3126,12 @@
       <c r="E119">
         <v>0</v>
       </c>
+      <c r="F119">
+        <v>1</v>
+      </c>
+      <c r="G119">
+        <v>0</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="str">
@@ -2435,6 +3149,12 @@
       <c r="E120">
         <v>0</v>
       </c>
+      <c r="F120">
+        <v>13</v>
+      </c>
+      <c r="G120">
+        <v>1</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="str">
@@ -2450,7 +3170,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Thu-tuc-To-tung/Luat-thi-hanh-tam-giu-tam-giam-2015-298373.aspx</v>
       </c>
       <c r="E121">
-        <v>21</v>
+        <v>20</v>
+      </c>
+      <c r="F121">
+        <v>8</v>
+      </c>
+      <c r="G121">
+        <v>18</v>
       </c>
     </row>
     <row r="122">
@@ -2469,6 +3195,12 @@
       <c r="E122">
         <v>2</v>
       </c>
+      <c r="F122">
+        <v>8</v>
+      </c>
+      <c r="G122">
+        <v>13</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="str">
@@ -2486,6 +3218,12 @@
       <c r="E123">
         <v>0</v>
       </c>
+      <c r="F123">
+        <v>9</v>
+      </c>
+      <c r="G123">
+        <v>1</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="str">
@@ -2503,6 +3241,12 @@
       <c r="E124">
         <v>0</v>
       </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+      <c r="G124">
+        <v>1</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="str">
@@ -2520,6 +3264,12 @@
       <c r="E125">
         <v>3</v>
       </c>
+      <c r="F125">
+        <v>25</v>
+      </c>
+      <c r="G125">
+        <v>16</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="str">
@@ -2537,6 +3287,12 @@
       <c r="E126">
         <v>0</v>
       </c>
+      <c r="F126">
+        <v>34</v>
+      </c>
+      <c r="G126">
+        <v>118</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="str">
@@ -2554,6 +3310,12 @@
       <c r="E127">
         <v>0</v>
       </c>
+      <c r="F127">
+        <v>26</v>
+      </c>
+      <c r="G127">
+        <v>22</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="str">
@@ -2571,6 +3333,12 @@
       <c r="E128">
         <v>0</v>
       </c>
+      <c r="F128">
+        <v>4</v>
+      </c>
+      <c r="G128">
+        <v>0</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="str">
@@ -2588,6 +3356,12 @@
       <c r="E129">
         <v>7</v>
       </c>
+      <c r="F129">
+        <v>19</v>
+      </c>
+      <c r="G129">
+        <v>2</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="str">
@@ -2605,6 +3379,12 @@
       <c r="E130">
         <v>0</v>
       </c>
+      <c r="F130">
+        <v>15</v>
+      </c>
+      <c r="G130">
+        <v>0</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="str">
@@ -2622,6 +3402,12 @@
       <c r="E131">
         <v>2</v>
       </c>
+      <c r="F131">
+        <v>7</v>
+      </c>
+      <c r="G131">
+        <v>64</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="str">
@@ -2639,6 +3425,12 @@
       <c r="E132">
         <v>0</v>
       </c>
+      <c r="F132">
+        <v>1</v>
+      </c>
+      <c r="G132">
+        <v>0</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="str">
@@ -2656,6 +3448,12 @@
       <c r="E133">
         <v>2</v>
       </c>
+      <c r="F133">
+        <v>30</v>
+      </c>
+      <c r="G133">
+        <v>71</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="str">
@@ -2673,6 +3471,12 @@
       <c r="E134">
         <v>0</v>
       </c>
+      <c r="F134">
+        <v>8</v>
+      </c>
+      <c r="G134">
+        <v>5</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="str">
@@ -2690,6 +3494,12 @@
       <c r="E135">
         <v>0</v>
       </c>
+      <c r="F135">
+        <v>190</v>
+      </c>
+      <c r="G135">
+        <v>0</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="str">
@@ -2707,6 +3517,12 @@
       <c r="E136">
         <v>1</v>
       </c>
+      <c r="F136">
+        <v>14</v>
+      </c>
+      <c r="G136">
+        <v>9</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="str">
@@ -2724,6 +3540,12 @@
       <c r="E137">
         <v>0</v>
       </c>
+      <c r="F137">
+        <v>10</v>
+      </c>
+      <c r="G137">
+        <v>2</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="str">
@@ -2741,6 +3563,12 @@
       <c r="E138">
         <v>2</v>
       </c>
+      <c r="F138">
+        <v>3</v>
+      </c>
+      <c r="G138">
+        <v>0</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="str">
@@ -2758,6 +3586,12 @@
       <c r="E139">
         <v>1</v>
       </c>
+      <c r="F139">
+        <v>11</v>
+      </c>
+      <c r="G139">
+        <v>0</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="str">
@@ -2775,6 +3609,12 @@
       <c r="E140">
         <v>0</v>
       </c>
+      <c r="F140">
+        <v>9</v>
+      </c>
+      <c r="G140">
+        <v>0</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="str">
@@ -2792,6 +3632,12 @@
       <c r="E141">
         <v>0</v>
       </c>
+      <c r="F141">
+        <v>1</v>
+      </c>
+      <c r="G141">
+        <v>1</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="str">
@@ -2807,7 +3653,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Bo-may-hanh-chinh/Luat-Cong-an-nhan-dan-2014-260648.aspx</v>
       </c>
       <c r="E142">
-        <v>20</v>
+        <v>18</v>
+      </c>
+      <c r="F142">
+        <v>4</v>
+      </c>
+      <c r="G142">
+        <v>4</v>
       </c>
     </row>
     <row r="143">
@@ -2826,6 +3678,12 @@
       <c r="E143">
         <v>0</v>
       </c>
+      <c r="F143">
+        <v>11</v>
+      </c>
+      <c r="G143">
+        <v>0</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="str">
@@ -2843,6 +3701,12 @@
       <c r="E144">
         <v>0</v>
       </c>
+      <c r="F144">
+        <v>1</v>
+      </c>
+      <c r="G144">
+        <v>0</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="str">
@@ -2860,6 +3724,12 @@
       <c r="E145">
         <v>0</v>
       </c>
+      <c r="F145">
+        <v>23</v>
+      </c>
+      <c r="G145">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="str">
@@ -2877,6 +3747,12 @@
       <c r="E146">
         <v>0</v>
       </c>
+      <c r="F146">
+        <v>1</v>
+      </c>
+      <c r="G146">
+        <v>0</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="str">
@@ -2894,6 +3770,12 @@
       <c r="E147">
         <v>0</v>
       </c>
+      <c r="F147">
+        <v>7</v>
+      </c>
+      <c r="G147">
+        <v>1</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="str">
@@ -2911,6 +3793,12 @@
       <c r="E148">
         <v>2</v>
       </c>
+      <c r="F148">
+        <v>10</v>
+      </c>
+      <c r="G148">
+        <v>132</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="str">
@@ -2928,6 +3816,12 @@
       <c r="E149">
         <v>0</v>
       </c>
+      <c r="F149">
+        <v>9</v>
+      </c>
+      <c r="G149">
+        <v>6</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="str">
@@ -2945,6 +3839,12 @@
       <c r="E150">
         <v>3</v>
       </c>
+      <c r="F150">
+        <v>7</v>
+      </c>
+      <c r="G150">
+        <v>4</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="str">
@@ -2962,6 +3862,12 @@
       <c r="E151">
         <v>2</v>
       </c>
+      <c r="F151">
+        <v>4</v>
+      </c>
+      <c r="G151">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="str">
@@ -2979,6 +3885,12 @@
       <c r="E152">
         <v>0</v>
       </c>
+      <c r="F152">
+        <v>4</v>
+      </c>
+      <c r="G152">
+        <v>5</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="str">
@@ -2996,6 +3908,12 @@
       <c r="E153">
         <v>0</v>
       </c>
+      <c r="F153">
+        <v>17</v>
+      </c>
+      <c r="G153">
+        <v>2</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="str">
@@ -3013,6 +3931,12 @@
       <c r="E154">
         <v>0</v>
       </c>
+      <c r="F154">
+        <v>1</v>
+      </c>
+      <c r="G154">
+        <v>0</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="str">
@@ -3030,6 +3954,12 @@
       <c r="E155">
         <v>2</v>
       </c>
+      <c r="F155">
+        <v>9</v>
+      </c>
+      <c r="G155">
+        <v>7</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="str">
@@ -3047,6 +3977,12 @@
       <c r="E156">
         <v>0</v>
       </c>
+      <c r="F156">
+        <v>11</v>
+      </c>
+      <c r="G156">
+        <v>3</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="str">
@@ -3062,7 +3998,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Quyen-dan-su/Luat-Hon-nhan-va-gia-dinh-2014-238640.aspx</v>
       </c>
       <c r="E157">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="F157">
+        <v>1</v>
+      </c>
+      <c r="G157">
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -3081,6 +4023,12 @@
       <c r="E158">
         <v>0</v>
       </c>
+      <c r="F158">
+        <v>5</v>
+      </c>
+      <c r="G158">
+        <v>0</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="str">
@@ -3098,6 +4046,12 @@
       <c r="E159">
         <v>0</v>
       </c>
+      <c r="F159">
+        <v>12</v>
+      </c>
+      <c r="G159">
+        <v>0</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="str">
@@ -3115,6 +4069,12 @@
       <c r="E160">
         <v>0</v>
       </c>
+      <c r="F160">
+        <v>14</v>
+      </c>
+      <c r="G160">
+        <v>2</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="str">
@@ -3132,6 +4092,12 @@
       <c r="E161">
         <v>5</v>
       </c>
+      <c r="F161">
+        <v>2</v>
+      </c>
+      <c r="G161">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="str">
@@ -3149,6 +4115,12 @@
       <c r="E162">
         <v>10</v>
       </c>
+      <c r="F162">
+        <v>4</v>
+      </c>
+      <c r="G162">
+        <v>1</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="str">
@@ -3166,6 +4138,12 @@
       <c r="E163">
         <v>7</v>
       </c>
+      <c r="F163">
+        <v>5</v>
+      </c>
+      <c r="G163">
+        <v>0</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="str">
@@ -3183,6 +4161,12 @@
       <c r="E164">
         <v>0</v>
       </c>
+      <c r="F164">
+        <v>61</v>
+      </c>
+      <c r="G164">
+        <v>3</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="str">
@@ -3200,6 +4184,12 @@
       <c r="E165">
         <v>1</v>
       </c>
+      <c r="F165">
+        <v>13</v>
+      </c>
+      <c r="G165">
+        <v>4</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="str">
@@ -3217,6 +4207,12 @@
       <c r="E166">
         <v>2</v>
       </c>
+      <c r="F166">
+        <v>5</v>
+      </c>
+      <c r="G166">
+        <v>0</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="str">
@@ -3234,6 +4230,12 @@
       <c r="E167">
         <v>6</v>
       </c>
+      <c r="F167">
+        <v>6</v>
+      </c>
+      <c r="G167">
+        <v>2</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="str">
@@ -3251,6 +4253,12 @@
       <c r="E168">
         <v>0</v>
       </c>
+      <c r="F168">
+        <v>3</v>
+      </c>
+      <c r="G168">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="str">
@@ -3268,6 +4276,12 @@
       <c r="E169">
         <v>4</v>
       </c>
+      <c r="F169">
+        <v>1</v>
+      </c>
+      <c r="G169">
+        <v>0</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="str">
@@ -3285,6 +4299,12 @@
       <c r="E170">
         <v>0</v>
       </c>
+      <c r="F170">
+        <v>3</v>
+      </c>
+      <c r="G170">
+        <v>0</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="str">
@@ -3302,6 +4322,12 @@
       <c r="E171">
         <v>8</v>
       </c>
+      <c r="F171">
+        <v>10</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="str">
@@ -3319,6 +4345,12 @@
       <c r="E172">
         <v>0</v>
       </c>
+      <c r="F172">
+        <v>1</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="str">
@@ -3336,6 +4368,12 @@
       <c r="E173">
         <v>1</v>
       </c>
+      <c r="F173">
+        <v>35</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="str">
@@ -3353,6 +4391,12 @@
       <c r="E174">
         <v>0</v>
       </c>
+      <c r="F174">
+        <v>1</v>
+      </c>
+      <c r="G174">
+        <v>0</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="str">
@@ -3370,6 +4414,12 @@
       <c r="E175">
         <v>0</v>
       </c>
+      <c r="F175">
+        <v>8</v>
+      </c>
+      <c r="G175">
+        <v>0</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="str">
@@ -3387,6 +4437,12 @@
       <c r="E176">
         <v>18</v>
       </c>
+      <c r="F176">
+        <v>4</v>
+      </c>
+      <c r="G176">
+        <v>4</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="str">
@@ -3404,6 +4460,12 @@
       <c r="E177">
         <v>0</v>
       </c>
+      <c r="F177">
+        <v>1</v>
+      </c>
+      <c r="G177">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="str">
@@ -3421,6 +4483,12 @@
       <c r="E178">
         <v>0</v>
       </c>
+      <c r="F178">
+        <v>9</v>
+      </c>
+      <c r="G178">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="str">
@@ -3438,6 +4506,12 @@
       <c r="E179">
         <v>0</v>
       </c>
+      <c r="F179">
+        <v>2</v>
+      </c>
+      <c r="G179">
+        <v>0</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="str">
@@ -3455,6 +4529,12 @@
       <c r="E180">
         <v>0</v>
       </c>
+      <c r="F180">
+        <v>10</v>
+      </c>
+      <c r="G180">
+        <v>3</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="str">
@@ -3472,6 +4552,12 @@
       <c r="E181">
         <v>8</v>
       </c>
+      <c r="F181">
+        <v>4</v>
+      </c>
+      <c r="G181">
+        <v>1</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="str">
@@ -3489,6 +4575,12 @@
       <c r="E182">
         <v>0</v>
       </c>
+      <c r="F182">
+        <v>1</v>
+      </c>
+      <c r="G182">
+        <v>0</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="str">
@@ -3506,6 +4598,12 @@
       <c r="E183">
         <v>0</v>
       </c>
+      <c r="F183">
+        <v>6</v>
+      </c>
+      <c r="G183">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="str">
@@ -3523,6 +4621,12 @@
       <c r="E184">
         <v>0</v>
       </c>
+      <c r="F184">
+        <v>1</v>
+      </c>
+      <c r="G184">
+        <v>6</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="str">
@@ -3540,6 +4644,12 @@
       <c r="E185">
         <v>10</v>
       </c>
+      <c r="F185">
+        <v>8</v>
+      </c>
+      <c r="G185">
+        <v>4</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="str">
@@ -3555,7 +4665,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Vi-pham-hanh-chinh/Luat-xu-ly-vi-pham-hanh-chinh-2012-142766.aspx</v>
       </c>
       <c r="E186">
-        <v>78</v>
+        <v>0</v>
+      </c>
+      <c r="F186">
+        <v>8</v>
+      </c>
+      <c r="G186">
+        <v>21</v>
       </c>
     </row>
     <row r="187">
@@ -3574,6 +4690,12 @@
       <c r="E187">
         <v>0</v>
       </c>
+      <c r="F187">
+        <v>2</v>
+      </c>
+      <c r="G187">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="str">
@@ -3591,6 +4713,12 @@
       <c r="E188">
         <v>0</v>
       </c>
+      <c r="F188">
+        <v>11</v>
+      </c>
+      <c r="G188">
+        <v>0</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="str">
@@ -3608,6 +4736,12 @@
       <c r="E189">
         <v>0</v>
       </c>
+      <c r="F189">
+        <v>10</v>
+      </c>
+      <c r="G189">
+        <v>0</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="str">
@@ -3625,6 +4759,12 @@
       <c r="E190">
         <v>0</v>
       </c>
+      <c r="F190">
+        <v>4</v>
+      </c>
+      <c r="G190">
+        <v>0</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="str">
@@ -3642,6 +4782,12 @@
       <c r="E191">
         <v>2</v>
       </c>
+      <c r="F191">
+        <v>4</v>
+      </c>
+      <c r="G191">
+        <v>0</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="str">
@@ -3659,6 +4805,12 @@
       <c r="E192">
         <v>0</v>
       </c>
+      <c r="F192">
+        <v>3</v>
+      </c>
+      <c r="G192">
+        <v>0</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="str">
@@ -3676,6 +4828,12 @@
       <c r="E193">
         <v>0</v>
       </c>
+      <c r="F193">
+        <v>11</v>
+      </c>
+      <c r="G193">
+        <v>0</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="str">
@@ -3693,6 +4851,12 @@
       <c r="E194">
         <v>1</v>
       </c>
+      <c r="F194">
+        <v>9</v>
+      </c>
+      <c r="G194">
+        <v>0</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="str">
@@ -3710,6 +4874,12 @@
       <c r="E195">
         <v>9</v>
       </c>
+      <c r="F195">
+        <v>5</v>
+      </c>
+      <c r="G195">
+        <v>2</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="str">
@@ -3727,6 +4897,12 @@
       <c r="E196">
         <v>0</v>
       </c>
+      <c r="F196">
+        <v>3</v>
+      </c>
+      <c r="G196">
+        <v>0</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
@@ -3742,7 +4918,13 @@
         <v>https://thuvienphapluat.vn/van-ban/Tai-nguyen-Moi-truong/Luat-khoang-san-2010-115263.aspx</v>
       </c>
       <c r="E197">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="F197">
+        <v>9</v>
+      </c>
+      <c r="G197">
+        <v>63</v>
       </c>
     </row>
     <row r="198">
@@ -3761,6 +4943,12 @@
       <c r="E198">
         <v>0</v>
       </c>
+      <c r="F198">
+        <v>1</v>
+      </c>
+      <c r="G198">
+        <v>0</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
@@ -3778,6 +4966,12 @@
       <c r="E199">
         <v>0</v>
       </c>
+      <c r="F199">
+        <v>9</v>
+      </c>
+      <c r="G199">
+        <v>7</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
@@ -3795,6 +4989,12 @@
       <c r="E200">
         <v>0</v>
       </c>
+      <c r="F200">
+        <v>5</v>
+      </c>
+      <c r="G200">
+        <v>2</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
@@ -3812,6 +5012,12 @@
       <c r="E201">
         <v>0</v>
       </c>
+      <c r="F201">
+        <v>8</v>
+      </c>
+      <c r="G201">
+        <v>2</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
@@ -3829,6 +5035,12 @@
       <c r="E202">
         <v>0</v>
       </c>
+      <c r="F202">
+        <v>20</v>
+      </c>
+      <c r="G202">
+        <v>4</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="str">
@@ -3846,6 +5058,12 @@
       <c r="E203">
         <v>0</v>
       </c>
+      <c r="F203">
+        <v>1</v>
+      </c>
+      <c r="G203">
+        <v>0</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="str">
@@ -3863,6 +5081,12 @@
       <c r="E204">
         <v>0</v>
       </c>
+      <c r="F204">
+        <v>17</v>
+      </c>
+      <c r="G204">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
@@ -3880,6 +5104,12 @@
       <c r="E205">
         <v>1</v>
       </c>
+      <c r="F205">
+        <v>3</v>
+      </c>
+      <c r="G205">
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
@@ -3897,6 +5127,12 @@
       <c r="E206">
         <v>1</v>
       </c>
+      <c r="F206">
+        <v>4</v>
+      </c>
+      <c r="G206">
+        <v>2</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
@@ -3914,6 +5150,12 @@
       <c r="E207">
         <v>0</v>
       </c>
+      <c r="F207">
+        <v>8</v>
+      </c>
+      <c r="G207">
+        <v>2</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="str">
@@ -3931,6 +5173,12 @@
       <c r="E208">
         <v>0</v>
       </c>
+      <c r="F208">
+        <v>7</v>
+      </c>
+      <c r="G208">
+        <v>0</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="str">
@@ -3948,6 +5196,12 @@
       <c r="E209">
         <v>0</v>
       </c>
+      <c r="F209">
+        <v>1</v>
+      </c>
+      <c r="G209">
+        <v>0</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="str">
@@ -3965,6 +5219,12 @@
       <c r="E210">
         <v>10</v>
       </c>
+      <c r="F210">
+        <v>10</v>
+      </c>
+      <c r="G210">
+        <v>0</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="str">
@@ -3982,6 +5242,12 @@
       <c r="E211">
         <v>0</v>
       </c>
+      <c r="F211">
+        <v>5</v>
+      </c>
+      <c r="G211">
+        <v>0</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="str">
@@ -3999,6 +5265,12 @@
       <c r="E212">
         <v>0</v>
       </c>
+      <c r="F212">
+        <v>2</v>
+      </c>
+      <c r="G212">
+        <v>0</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="str">
@@ -4016,6 +5288,12 @@
       <c r="E213">
         <v>0</v>
       </c>
+      <c r="F213">
+        <v>6</v>
+      </c>
+      <c r="G213">
+        <v>0</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="str">
@@ -4033,6 +5311,12 @@
       <c r="E214">
         <v>0</v>
       </c>
+      <c r="F214">
+        <v>3</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="str">
@@ -4050,6 +5334,12 @@
       <c r="E215">
         <v>8</v>
       </c>
+      <c r="F215">
+        <v>4</v>
+      </c>
+      <c r="G215">
+        <v>1</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="str">
@@ -4067,6 +5357,12 @@
       <c r="E216">
         <v>0</v>
       </c>
+      <c r="F216">
+        <v>10</v>
+      </c>
+      <c r="G216">
+        <v>1</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="str">
@@ -4084,6 +5380,12 @@
       <c r="E217">
         <v>0</v>
       </c>
+      <c r="F217">
+        <v>3</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="str">
@@ -4101,6 +5403,12 @@
       <c r="E218">
         <v>1</v>
       </c>
+      <c r="F218">
+        <v>11</v>
+      </c>
+      <c r="G218">
+        <v>1</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="str">
@@ -4118,6 +5426,12 @@
       <c r="E219">
         <v>0</v>
       </c>
+      <c r="F219">
+        <v>1</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="str">
@@ -4135,6 +5449,12 @@
       <c r="E220">
         <v>0</v>
       </c>
+      <c r="F220">
+        <v>4</v>
+      </c>
+      <c r="G220">
+        <v>19</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="str">
@@ -4152,6 +5472,12 @@
       <c r="E221">
         <v>0</v>
       </c>
+      <c r="F221">
+        <v>9</v>
+      </c>
+      <c r="G221">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="str">
@@ -4169,6 +5495,12 @@
       <c r="E222">
         <v>0</v>
       </c>
+      <c r="F222">
+        <v>3</v>
+      </c>
+      <c r="G222">
+        <v>5</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="str">
@@ -4186,6 +5518,12 @@
       <c r="E223">
         <v>9</v>
       </c>
+      <c r="F223">
+        <v>2</v>
+      </c>
+      <c r="G223">
+        <v>1</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="str">
@@ -4203,6 +5541,12 @@
       <c r="E224">
         <v>2</v>
       </c>
+      <c r="F224">
+        <v>2</v>
+      </c>
+      <c r="G224">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="str">
@@ -4220,6 +5564,12 @@
       <c r="E225">
         <v>0</v>
       </c>
+      <c r="F225">
+        <v>5</v>
+      </c>
+      <c r="G225">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="str">
@@ -4237,6 +5587,12 @@
       <c r="E226">
         <v>0</v>
       </c>
+      <c r="F226">
+        <v>1</v>
+      </c>
+      <c r="G226">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="str">
@@ -4254,6 +5610,12 @@
       <c r="E227">
         <v>2</v>
       </c>
+      <c r="F227">
+        <v>6</v>
+      </c>
+      <c r="G227">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="str">
@@ -4271,6 +5633,12 @@
       <c r="E228">
         <v>1</v>
       </c>
+      <c r="F228">
+        <v>4</v>
+      </c>
+      <c r="G228">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="str">
@@ -4288,6 +5656,12 @@
       <c r="E229">
         <v>0</v>
       </c>
+      <c r="F229">
+        <v>1</v>
+      </c>
+      <c r="G229">
+        <v>0</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="str">
@@ -4305,6 +5679,12 @@
       <c r="E230">
         <v>2</v>
       </c>
+      <c r="F230">
+        <v>1</v>
+      </c>
+      <c r="G230">
+        <v>4</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="str">
@@ -4322,6 +5702,12 @@
       <c r="E231">
         <v>0</v>
       </c>
+      <c r="F231">
+        <v>1</v>
+      </c>
+      <c r="G231">
+        <v>0</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="str">
@@ -4339,6 +5725,12 @@
       <c r="E232">
         <v>0</v>
       </c>
+      <c r="F232">
+        <v>6</v>
+      </c>
+      <c r="G232">
+        <v>0</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="str">
@@ -4356,6 +5748,12 @@
       <c r="E233">
         <v>0</v>
       </c>
+      <c r="F233">
+        <v>4</v>
+      </c>
+      <c r="G233">
+        <v>0</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="str">
@@ -4373,6 +5771,12 @@
       <c r="E234">
         <v>0</v>
       </c>
+      <c r="F234">
+        <v>2</v>
+      </c>
+      <c r="G234">
+        <v>0</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="str">
@@ -4390,6 +5794,12 @@
       <c r="E235">
         <v>1</v>
       </c>
+      <c r="F235">
+        <v>20</v>
+      </c>
+      <c r="G235">
+        <v>1</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="str">
@@ -4407,6 +5817,12 @@
       <c r="E236">
         <v>28</v>
       </c>
+      <c r="F236">
+        <v>1</v>
+      </c>
+      <c r="G236">
+        <v>16</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="str">
@@ -4424,6 +5840,12 @@
       <c r="E237">
         <v>1</v>
       </c>
+      <c r="F237">
+        <v>8</v>
+      </c>
+      <c r="G237">
+        <v>0</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="str">
@@ -4441,6 +5863,12 @@
       <c r="E238">
         <v>0</v>
       </c>
+      <c r="F238">
+        <v>5</v>
+      </c>
+      <c r="G238">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="str">
@@ -4458,6 +5886,12 @@
       <c r="E239">
         <v>2</v>
       </c>
+      <c r="F239">
+        <v>2</v>
+      </c>
+      <c r="G239">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="str">
@@ -4475,6 +5909,12 @@
       <c r="E240">
         <v>0</v>
       </c>
+      <c r="F240">
+        <v>54</v>
+      </c>
+      <c r="G240">
+        <v>0</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="str">
@@ -4492,6 +5932,12 @@
       <c r="E241">
         <v>0</v>
       </c>
+      <c r="F241">
+        <v>5</v>
+      </c>
+      <c r="G241">
+        <v>1</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="str">
@@ -4509,6 +5955,12 @@
       <c r="E242">
         <v>0</v>
       </c>
+      <c r="F242">
+        <v>8</v>
+      </c>
+      <c r="G242">
+        <v>4</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="str">
@@ -4526,6 +5978,12 @@
       <c r="E243">
         <v>2</v>
       </c>
+      <c r="F243">
+        <v>4</v>
+      </c>
+      <c r="G243">
+        <v>23</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="str">
@@ -4543,6 +6001,12 @@
       <c r="E244">
         <v>2</v>
       </c>
+      <c r="F244">
+        <v>0</v>
+      </c>
+      <c r="G244">
+        <v>3</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="str">
@@ -4560,6 +6024,12 @@
       <c r="E245">
         <v>0</v>
       </c>
+      <c r="F245">
+        <v>4</v>
+      </c>
+      <c r="G245">
+        <v>0</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="str">
@@ -4577,6 +6047,12 @@
       <c r="E246">
         <v>0</v>
       </c>
+      <c r="F246">
+        <v>0</v>
+      </c>
+      <c r="G246">
+        <v>0</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="str">
@@ -4594,6 +6070,12 @@
       <c r="E247">
         <v>0</v>
       </c>
+      <c r="F247">
+        <v>0</v>
+      </c>
+      <c r="G247">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="str">
@@ -4611,6 +6093,12 @@
       <c r="E248">
         <v>0</v>
       </c>
+      <c r="F248">
+        <v>0</v>
+      </c>
+      <c r="G248">
+        <v>0</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="str">
@@ -4628,6 +6116,12 @@
       <c r="E249">
         <v>5</v>
       </c>
+      <c r="F249">
+        <v>1</v>
+      </c>
+      <c r="G249">
+        <v>1</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="str">
@@ -4645,6 +6139,12 @@
       <c r="E250">
         <v>1</v>
       </c>
+      <c r="F250">
+        <v>3</v>
+      </c>
+      <c r="G250">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="str">
@@ -4662,6 +6162,12 @@
       <c r="E251">
         <v>7</v>
       </c>
+      <c r="F251">
+        <v>0</v>
+      </c>
+      <c r="G251">
+        <v>3</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="str">
@@ -4679,6 +6185,12 @@
       <c r="E252">
         <v>0</v>
       </c>
+      <c r="F252">
+        <v>1</v>
+      </c>
+      <c r="G252">
+        <v>0</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="str">
@@ -4696,6 +6208,12 @@
       <c r="E253">
         <v>1</v>
       </c>
+      <c r="F253">
+        <v>1</v>
+      </c>
+      <c r="G253">
+        <v>0</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="str">
@@ -4713,6 +6231,12 @@
       <c r="E254">
         <v>0</v>
       </c>
+      <c r="F254">
+        <v>3</v>
+      </c>
+      <c r="G254">
+        <v>0</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="str">
@@ -4730,6 +6254,12 @@
       <c r="E255">
         <v>0</v>
       </c>
+      <c r="F255">
+        <v>2</v>
+      </c>
+      <c r="G255">
+        <v>0</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="str">
@@ -4747,6 +6277,12 @@
       <c r="E256">
         <v>0</v>
       </c>
+      <c r="F256">
+        <v>0</v>
+      </c>
+      <c r="G256">
+        <v>1</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="str">
@@ -4764,6 +6300,12 @@
       <c r="E257">
         <v>0</v>
       </c>
+      <c r="F257">
+        <v>2</v>
+      </c>
+      <c r="G257">
+        <v>0</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="str">
@@ -4781,6 +6323,12 @@
       <c r="E258">
         <v>0</v>
       </c>
+      <c r="F258">
+        <v>1</v>
+      </c>
+      <c r="G258">
+        <v>0</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="str">
@@ -4798,10 +6346,16 @@
       <c r="E259">
         <v>0</v>
       </c>
+      <c r="F259">
+        <v>1</v>
+      </c>
+      <c r="G259">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E259"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:G259"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>